<commit_message>
Delete Post, User Wall & Friends Posts , Comments functionality added, Bugs Fixed, News Feed Page implemented
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="0" windowWidth="23040" windowHeight="9405"/>
+    <workbookView xWindow="2220" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>GitHub (up to 100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>GithHub Profile Link</t>
@@ -644,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +654,7 @@
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>10</v>
@@ -666,12 +663,12 @@
         <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -679,20 +676,20 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -707,7 +704,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -717,9 +714,11 @@
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>9</v>
+      </c>
       <c r="D8" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="6"/>
     </row>
@@ -727,15 +726,17 @@
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>15</v>
+      </c>
       <c r="D9" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -745,8 +746,8 @@
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>12</v>
+      <c r="C11" s="5">
+        <v>7</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
@@ -757,7 +758,9 @@
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5">
+        <v>30</v>
+      </c>
       <c r="D12" s="5">
         <v>30</v>
       </c>
@@ -767,7 +770,9 @@
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5">
+        <v>5</v>
+      </c>
       <c r="D13" s="5">
         <v>5</v>
       </c>
@@ -775,9 +780,11 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="C14" s="5">
+        <v>10</v>
+      </c>
       <c r="D14" s="5">
         <v>10</v>
       </c>
@@ -787,7 +794,9 @@
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5">
+        <v>5</v>
+      </c>
       <c r="D15" s="5">
         <v>5</v>
       </c>
@@ -795,9 +804,11 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="C16" s="5">
+        <v>10</v>
+      </c>
       <c r="D16" s="5">
         <v>10</v>
       </c>
@@ -805,9 +816,11 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3</v>
+      </c>
       <c r="D17" s="5">
         <v>3</v>
       </c>
@@ -815,9 +828,11 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="C18" s="5">
+        <v>7</v>
+      </c>
       <c r="D18" s="5">
         <v>7</v>
       </c>
@@ -825,9 +840,11 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="C19" s="5">
+        <v>10</v>
+      </c>
       <c r="D19" s="5">
         <v>10</v>
       </c>
@@ -835,9 +852,11 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
       <c r="D20" s="5">
         <v>5</v>
       </c>
@@ -845,9 +864,11 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="C21" s="5">
+        <v>10</v>
+      </c>
       <c r="D21" s="5">
         <v>10</v>
       </c>
@@ -855,9 +876,11 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="C22" s="5">
+        <v>10</v>
+      </c>
       <c r="D22" s="5">
         <v>10</v>
       </c>
@@ -865,9 +888,11 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="C23" s="5">
+        <v>5</v>
+      </c>
       <c r="D23" s="5">
         <v>5</v>
       </c>
@@ -875,7 +900,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5">
@@ -885,9 +910,11 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="C25" s="5">
+        <v>10</v>
+      </c>
       <c r="D25" s="5">
         <v>10</v>
       </c>
@@ -895,9 +922,11 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="C26" s="5">
+        <v>10</v>
+      </c>
       <c r="D26" s="5">
         <v>10</v>
       </c>
@@ -905,9 +934,11 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C27" s="5">
+        <v>10</v>
+      </c>
       <c r="D27" s="5">
         <v>10</v>
       </c>
@@ -915,7 +946,7 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5">
@@ -925,9 +956,11 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="C29" s="5">
+        <v>5</v>
+      </c>
       <c r="D29" s="5">
         <v>5</v>
       </c>
@@ -937,7 +970,9 @@
       <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5">
+        <v>10</v>
+      </c>
       <c r="D30" s="5">
         <v>10</v>
       </c>
@@ -945,9 +980,11 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C31" s="5">
+        <v>5</v>
+      </c>
       <c r="D31" s="5">
         <v>5</v>
       </c>
@@ -957,7 +994,9 @@
       <c r="B32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5">
+        <v>5</v>
+      </c>
       <c r="D32" s="5">
         <v>5</v>
       </c>
@@ -965,9 +1004,11 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C33" s="5">
+        <v>5</v>
+      </c>
       <c r="D33" s="5">
         <v>5</v>
       </c>
@@ -975,9 +1016,11 @@
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C34" s="5">
+        <v>10</v>
+      </c>
       <c r="D34" s="5">
         <v>10</v>
       </c>
@@ -985,7 +1028,7 @@
     </row>
     <row r="35" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B35" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
@@ -993,7 +1036,7 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7">
@@ -1003,7 +1046,7 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7">
@@ -1013,7 +1056,7 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7">
@@ -1023,7 +1066,7 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7">
@@ -1033,7 +1076,7 @@
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7">
@@ -1043,7 +1086,7 @@
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7">
@@ -1053,9 +1096,11 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="C42" s="7">
+        <v>20</v>
+      </c>
       <c r="D42" s="7">
         <v>20</v>
       </c>
@@ -1063,7 +1108,7 @@
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7">
@@ -1077,7 +1122,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>

<commit_message>
Delete Post Comment, Edit Post ADDED
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="0" windowWidth="23040" windowHeight="9405"/>
+    <workbookView xWindow="3330" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -641,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -948,7 +948,9 @@
       <c r="B28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
       <c r="D28" s="5">
         <v>5</v>
       </c>
@@ -1088,7 +1090,9 @@
       <c r="B41" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="7">
+        <v>5</v>
+      </c>
       <c r="D41" s="7">
         <v>5</v>
       </c>
@@ -1122,7 +1126,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>

<commit_message>
Edit Comment Added to List
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="0" windowWidth="23040" windowHeight="9405"/>
+    <workbookView xWindow="4440" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -642,7 +642,7 @@
   <dimension ref="B2:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1080,9 @@
       <c r="B40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="7">
+        <v>5</v>
+      </c>
       <c r="D40" s="7">
         <v>5</v>
       </c>
@@ -1126,7 +1128,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>